<commit_message>
Data Provider,Data Provider Utility
</commit_message>
<xml_diff>
--- a/testDataTr/LogInTr.xlsx
+++ b/testDataTr/LogInTr.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">heet.n@inheritx.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tourwitqa@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -59,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -88,6 +91,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,6 +155,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,10 +351,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -400,7 +413,18 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -408,6 +432,8 @@
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" display="heet.n@inheritx.com"/>
     <hyperlink ref="B5" r:id="rId2" display="Test@123"/>
+    <hyperlink ref="A6" r:id="rId3" display="tourwitqa@yopmail.com"/>
+    <hyperlink ref="B6" r:id="rId4" display="Test@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>